<commit_message>
test/fix: * Added a bunch of test cases and updated the verification matrix. Also added a TestAdapter and adapted the code a bit to make it testable. * Fixed some small bugs in the code discovered when running the test cases - nothing serious though.
</commit_message>
<xml_diff>
--- a/Test/VerificationMatrix.xlsx
+++ b/Test/VerificationMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Components\GECKO\Gecko3\GECKO\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49EB212-86EA-47E3-B9C6-A3B5129CB5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8991210D-20B2-4784-ABD8-497C472A2238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
   <si>
     <t>Verification</t>
   </si>
@@ -208,6 +209,39 @@
   </si>
   <si>
     <t>userdata/ecYeastGEM/code/sumProtein.m</t>
+  </si>
+  <si>
+    <t>saveECModel.m</t>
+  </si>
+  <si>
+    <t>enhanceGEM.m</t>
+  </si>
+  <si>
+    <t>Probably not relevant anymore, remove?</t>
+  </si>
+  <si>
+    <t>tc0001, tc0002</t>
+  </si>
+  <si>
+    <t>tc0003, tc0004 - File download not covered by test cases but is tested manually and works.</t>
+  </si>
+  <si>
+    <t>tc0005</t>
+  </si>
+  <si>
+    <t>tc0003, tc0004</t>
+  </si>
+  <si>
+    <t>tc0006</t>
+  </si>
+  <si>
+    <t>tc0007 - does not test download of the databases - this is tested in the manual workflows for Yeast-GEM and Human-GEM</t>
+  </si>
+  <si>
+    <t>tc0008</t>
+  </si>
+  <si>
+    <t>tc0009 - currently doesn't work</t>
   </si>
 </sst>
 </file>
@@ -534,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,6 +600,9 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -581,16 +618,25 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -642,11 +688,17 @@
       <c r="A17" t="s">
         <v>16</v>
       </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -798,6 +850,9 @@
       <c r="A41" t="s">
         <v>47</v>
       </c>
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
@@ -849,7 +904,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -857,7 +912,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -865,12 +920,31 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>60</v>
       </c>
       <c r="B51" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
doc: Updated verification matrix
</commit_message>
<xml_diff>
--- a/Test/VerificationMatrix.xlsx
+++ b/Test/VerificationMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Components\GECKO\Gecko3\GECKO\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8991210D-20B2-4784-ABD8-497C472A2238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A86224-BE9A-44D9-AD30-85A09B9CAC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
   <si>
     <t>Verification</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>tc0009 - currently doesn't work</t>
+  </si>
+  <si>
+    <t>tc0010</t>
   </si>
 </sst>
 </file>
@@ -571,7 +574,7 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,6 +645,9 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">

</xml_diff>